<commit_message>
started with error code
</commit_message>
<xml_diff>
--- a/Group25 DBL Scrum Timesheets.xlsx
+++ b/Group25 DBL Scrum Timesheets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G\Documents\Documenten TU-Eindhoven\Year 1 - Q4\DBL C++\Github\Embedded_system_group25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD8A2AE-D374-4B2E-AC62-8A5DE5104E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399B3BDA-F0F6-4AB0-A6B9-2FE297042B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="222">
   <si>
     <t>Project:</t>
   </si>
@@ -711,6 +711,9 @@
   <si>
     <t>fixing timesheet</t>
   </si>
+  <si>
+    <t>coding error handling</t>
+  </si>
 </sst>
 </file>
 
@@ -1167,7 +1170,7 @@
                 <c:formatCode>[h]:mm</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2.3305555555555553</c:v>
+                  <c:v>2.3930555555555553</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.95833333333333337</c:v>
@@ -1426,7 +1429,7 @@
                   <c:v>1.1875</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.70833333333333337</c:v>
+                  <c:v>0.77083333333333337</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1465,7 +1468,7 @@
                   <c:v>1.1875</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.70833333333333337</c:v>
+                  <c:v>0.77083333333333337</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -2041,10 +2044,10 @@
                   <c:v>0.22916666666666669</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.25</c:v>
+                  <c:v>0.27083333333333331</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>4.1666666666666664E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>3.125E-2</c:v>
@@ -4327,7 +4330,7 @@
   <dimension ref="A1:X1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4907,7 +4910,9 @@
       <c r="F22" s="43"/>
       <c r="G22" s="43"/>
       <c r="H22" s="43"/>
-      <c r="I22" s="43"/>
+      <c r="I22" s="43">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="J22" s="43"/>
       <c r="K22" s="43"/>
       <c r="L22" s="43"/>
@@ -4923,14 +4928,18 @@
       <c r="X22" s="38"/>
     </row>
     <row r="23" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>221</v>
+      </c>
       <c r="C23" s="10"/>
       <c r="D23" s="11"/>
       <c r="E23" s="43"/>
       <c r="F23" s="43"/>
       <c r="G23" s="43"/>
       <c r="H23" s="43"/>
-      <c r="I23" s="43"/>
+      <c r="I23" s="43">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="J23" s="43"/>
       <c r="K23" s="43"/>
       <c r="L23" s="43"/>
@@ -7440,7 +7449,7 @@
       </c>
       <c r="I128" s="45">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>0.1875</v>
       </c>
       <c r="J128" s="45">
         <f t="shared" si="0"/>
@@ -7509,19 +7518,19 @@
       </c>
       <c r="I130" s="38">
         <f>SUM(C128:I128)</f>
-        <v>2.3305555555555553</v>
+        <v>2.3930555555555553</v>
       </c>
       <c r="J130" s="38">
         <f>SUM(C128:J128)</f>
-        <v>2.3305555555555553</v>
+        <v>2.3930555555555553</v>
       </c>
       <c r="K130" s="38">
         <f>SUM(C128:K128)</f>
-        <v>2.3305555555555553</v>
+        <v>2.3930555555555553</v>
       </c>
       <c r="L130" s="38">
         <f>SUM(C128:L128)</f>
-        <v>2.3305555555555553</v>
+        <v>2.3930555555555553</v>
       </c>
       <c r="M130" s="46"/>
       <c r="O130" s="38"/>
@@ -7565,19 +7574,19 @@
       </c>
       <c r="I131" s="38">
         <f>Parameters!$G$9-I130</f>
-        <v>3.5027777777777778</v>
+        <v>3.4402777777777778</v>
       </c>
       <c r="J131" s="38">
         <f>Parameters!$G$9-J130</f>
-        <v>3.5027777777777778</v>
+        <v>3.4402777777777778</v>
       </c>
       <c r="K131" s="38">
         <f>Parameters!$G$9-K130</f>
-        <v>3.5027777777777778</v>
+        <v>3.4402777777777778</v>
       </c>
       <c r="L131" s="38">
         <f>Parameters!$G$9-L130</f>
-        <v>3.5027777777777778</v>
+        <v>3.4402777777777778</v>
       </c>
       <c r="O131" s="38"/>
       <c r="P131" s="38"/>
@@ -29977,7 +29986,7 @@
       </c>
       <c r="I22" s="47">
         <f>SUM('Serkan Efe Durusu'!I22,'Ismail Elmasry'!I22,'can Işmar'!I22,'Marios Papalouka'!I22,'Metehan Topaç'!I22,'Celine Zanders '!I22)</f>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="J22" s="47">
         <f>SUM('Serkan Efe Durusu'!J22,'Ismail Elmasry'!J22,'can Işmar'!J22,'Marios Papalouka'!J22,'Metehan Topaç'!J22,'Celine Zanders '!J22)</f>
@@ -29993,7 +30002,7 @@
       </c>
       <c r="M22" s="50">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>0.27083333333333331</v>
       </c>
       <c r="N22" s="49" t="str">
         <f t="array" ref="N22">IF(INDEX(Tasks,1,3)&lt;&gt;"",100*M22/INDEX(Tasks,1,3),"")</f>
@@ -30031,7 +30040,7 @@
       </c>
       <c r="I23" s="47">
         <f>SUM('Serkan Efe Durusu'!I23,'Ismail Elmasry'!I23,'can Işmar'!I23,'Marios Papalouka'!I23,'Metehan Topaç'!I23,'Celine Zanders '!I23)</f>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="J23" s="47">
         <f>SUM('Serkan Efe Durusu'!J23,'Ismail Elmasry'!J23,'can Işmar'!J23,'Marios Papalouka'!J23,'Metehan Topaç'!J23,'Celine Zanders '!J23)</f>
@@ -30047,7 +30056,7 @@
       </c>
       <c r="M23" s="50">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="N23" s="49" t="str">
         <f t="array" ref="N23">IF(INDEX(Tasks,2,3)&lt;&gt;"",100*M23/INDEX(Tasks,2,3),"")</f>
@@ -35479,7 +35488,7 @@
       </c>
       <c r="I135" s="43">
         <f>'Serkan Efe Durusu'!I128</f>
-        <v>0.125</v>
+        <v>0.1875</v>
       </c>
       <c r="J135" s="43">
         <f>'Serkan Efe Durusu'!J128</f>
@@ -35495,7 +35504,7 @@
       </c>
       <c r="M135" s="53">
         <f t="shared" ref="M135:M143" si="1">SUM(C135:L135)</f>
-        <v>2.3305555555555553</v>
+        <v>2.3930555555555553</v>
       </c>
     </row>
     <row r="136" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -35855,7 +35864,7 @@
       </c>
       <c r="I143" s="53">
         <f t="shared" si="2"/>
-        <v>0.70833333333333337</v>
+        <v>0.77083333333333337</v>
       </c>
       <c r="J143" s="53">
         <f t="shared" si="2"/>
@@ -35871,7 +35880,7 @@
       </c>
       <c r="M143" s="53">
         <f t="shared" si="1"/>
-        <v>11.28888888888889</v>
+        <v>11.35138888888889</v>
       </c>
     </row>
     <row r="144" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>